<commit_message>
Refactor: centralize return file eligibility check and fix download path to use artifacts folder
</commit_message>
<xml_diff>
--- a/src/data/TestData.xlsx
+++ b/src/data/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RC-BatchFile-Automation Folder\RCAutomation-16Jan2026\RC-Smoke\RCBatch\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcharles\source\Repository\CDBatch_Migration\RC_Partial\RCBatch\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C458043E-278E-48C4-A0CC-0415EA29ED7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8104980C-A360-459A-ACC0-8952D43EEC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
   <si>
     <t>ScenarioId</t>
   </si>
@@ -171,6 +171,27 @@
   </si>
   <si>
     <t>AmendmentFileDescription</t>
+  </si>
+  <si>
+    <t>TDAF</t>
+  </si>
+  <si>
+    <t>TDAF Daily Input XIF File</t>
+  </si>
+  <si>
+    <t>TDAF_Renewal</t>
+  </si>
+  <si>
+    <t>TDAF Daily Input Renewal CSV File</t>
+  </si>
+  <si>
+    <t>TDAF_HappyPath_NF</t>
+  </si>
+  <si>
+    <t>TDAF_NF</t>
+  </si>
+  <si>
+    <t>TDAF Daily NF Output XML File</t>
   </si>
 </sst>
 </file>
@@ -220,7 +241,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -537,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,18 +817,50 @@
         <v>31</v>
       </c>
     </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" t="s">
+        <v>50</v>
+      </c>
+      <c r="P8" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:V2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A1:A2 A8:A1048576">
+  <conditionalFormatting sqref="A1:A2 A9:A1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
+  <conditionalFormatting sqref="A4">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
+  <conditionalFormatting sqref="A5:A7">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A7">
+  <conditionalFormatting sqref="A8">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>